<commit_message>
backup functional hicpro 2.11.1
</commit_message>
<xml_diff>
--- a/datahub_maker/extra_data.xlsx
+++ b/datahub_maker/extra_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A0D2CB-4C63-4359-89D8-242F579125E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE1A742-3879-456B-8B49-A8634A96C751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="-98" windowWidth="27795" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1087" yWindow="-98" windowWidth="27811" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="264">
   <si>
     <t>type</t>
   </si>
@@ -809,6 +809,18 @@
   </si>
   <si>
     <t>JIA_elena_suggestive_hg38</t>
+  </si>
+  <si>
+    <t>JIA_merged_HiC</t>
+  </si>
+  <si>
+    <t>JIA_merged_pCHiC</t>
+  </si>
+  <si>
+    <t>http://bartzabel.ls.manchester.ac.uk/worthingtonlab/psa_functional_genomics/JIA_CHiC/jia_hic_merged_MBOI.allValidPairs.hic</t>
+  </si>
+  <si>
+    <t>http://bartzabel.ls.manchester.ac.uk/worthingtonlab/psa_functional_genomics/JIA_CHiC/jia_merged_washU_text.txt.new_washu.bed.gz</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2585,6 +2597,34 @@
         <v>257</v>
       </c>
       <c r="D101" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" t="s">
+        <v>260</v>
+      </c>
+      <c r="C102" t="s">
+        <v>262</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B103" t="s">
+        <v>261</v>
+      </c>
+      <c r="C103" t="s">
+        <v>263</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>251</v>
       </c>
     </row>

</xml_diff>